<commit_message>
updated survey reports with two new stakeholders
git-svn-id: https://asi-storage07.blr.allegisindia.com/svn/EASi_App-POC@73 56ebe14e-9609-f449-8404-ff2adf786831
</commit_message>
<xml_diff>
--- a/trunk/EasiCab/Documents/Planning/Survey Reports.xlsx
+++ b/trunk/EasiCab/Documents/Planning/Survey Reports.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="60">
   <si>
     <t xml:space="preserve">Name: </t>
   </si>
@@ -114,9 +114,6 @@
   </si>
   <si>
     <t>91-8030705446</t>
-  </si>
-  <si>
-    <t>In puts:</t>
   </si>
   <si>
     <r>
@@ -196,6 +193,21 @@
   </si>
   <si>
     <t>Survey Report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In puts: </t>
+  </si>
+  <si>
+    <t>introduce two team members, Will planned to have meetingson 25 august 2016</t>
+  </si>
+  <si>
+    <t>mchintha@easi.com</t>
+  </si>
+  <si>
+    <t>email:</t>
+  </si>
+  <si>
+    <t>hmanohor@easi.com</t>
   </si>
 </sst>
 </file>
@@ -594,7 +606,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
@@ -627,8 +639,60 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="15" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -637,11 +701,38 @@
     <xf numFmtId="14" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -651,89 +742,16 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1122,7 +1140,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
@@ -1579,121 +1597,121 @@
       <c r="N4" s="17"/>
     </row>
     <row r="5" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" s="53"/>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="53"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="53"/>
-      <c r="K5" s="53"/>
-      <c r="L5" s="53"/>
-      <c r="M5" s="53"/>
+      <c r="A5" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
       <c r="N5" s="20"/>
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="19"/>
+    </row>
+    <row r="7" spans="1:14" s="21" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="26"/>
+    </row>
+    <row r="8" spans="1:14" s="21" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="54" t="s">
-        <v>54</v>
-      </c>
-      <c r="G6" s="54"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="54"/>
-      <c r="K6" s="54"/>
-      <c r="L6" s="54"/>
-      <c r="M6" s="54"/>
-      <c r="N6" s="19"/>
-    </row>
-    <row r="7" spans="1:14" s="21" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="41" t="s">
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="55" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
-      <c r="K7" s="55"/>
-      <c r="L7" s="55"/>
-      <c r="M7" s="55"/>
-      <c r="N7" s="26"/>
-    </row>
-    <row r="8" spans="1:14" s="21" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="41" t="s">
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="34"/>
+      <c r="M8" s="35"/>
+      <c r="N8" s="25"/>
+    </row>
+    <row r="9" spans="1:14" s="21" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="42"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="43" t="s">
-        <v>50</v>
-      </c>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="43"/>
-      <c r="L8" s="43"/>
-      <c r="M8" s="44"/>
-      <c r="N8" s="25"/>
-    </row>
-    <row r="9" spans="1:14" s="21" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="42"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="43">
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="34">
         <v>1</v>
       </c>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="43"/>
-      <c r="L9" s="43"/>
-      <c r="M9" s="44"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="34"/>
+      <c r="M9" s="35"/>
       <c r="N9" s="25"/>
     </row>
     <row r="10" spans="1:14" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="45" t="s">
+      <c r="A10" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="46"/>
-      <c r="K10" s="46"/>
-      <c r="L10" s="46"/>
-      <c r="M10" s="46"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="37"/>
+      <c r="M10" s="37"/>
       <c r="N10" s="24"/>
     </row>
     <row r="11" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -1745,126 +1763,121 @@
       <c r="N13" s="23"/>
     </row>
     <row r="14" spans="1:14" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="47" t="s">
+      <c r="A14" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="39"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="39"/>
+      <c r="F14" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="48"/>
-      <c r="C14" s="48"/>
-      <c r="D14" s="49" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" s="48"/>
-      <c r="F14" s="49" t="s">
+      <c r="J14" s="41"/>
+      <c r="K14" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="L14" s="42"/>
+      <c r="M14" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="N14" s="44"/>
+    </row>
+    <row r="15" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="47">
+        <v>1</v>
+      </c>
+      <c r="B15" s="48"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="49">
+        <v>42600</v>
+      </c>
+      <c r="E15" s="48"/>
+      <c r="F15" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="48"/>
-      <c r="H14" s="48"/>
-      <c r="I14" s="49" t="s">
-        <v>39</v>
-      </c>
-      <c r="J14" s="50"/>
-      <c r="K14" s="49" t="s">
-        <v>40</v>
-      </c>
-      <c r="L14" s="51"/>
-      <c r="M14" s="64" t="s">
-        <v>46</v>
-      </c>
-      <c r="N14" s="65"/>
-    </row>
-    <row r="15" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="29">
-        <v>1</v>
-      </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="31">
-        <v>42600</v>
-      </c>
-      <c r="E15" s="30"/>
-      <c r="F15" s="38" t="s">
-        <v>45</v>
-      </c>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="39" t="s">
-        <v>53</v>
-      </c>
-      <c r="J15" s="40"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="32"/>
-      <c r="M15" s="62" t="s">
+      <c r="G15" s="51"/>
+      <c r="H15" s="51"/>
+      <c r="I15" s="52" t="s">
         <v>52</v>
       </c>
-      <c r="N15" s="63"/>
+      <c r="J15" s="53"/>
+      <c r="K15" s="54"/>
+      <c r="L15" s="54"/>
+      <c r="M15" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="N15" s="56"/>
     </row>
     <row r="16" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="29"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
-      <c r="M16" s="60"/>
-      <c r="N16" s="61"/>
+      <c r="A16" s="47"/>
+      <c r="B16" s="48"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="51"/>
+      <c r="H16" s="51"/>
+      <c r="I16" s="54"/>
+      <c r="J16" s="54"/>
+      <c r="K16" s="54"/>
+      <c r="L16" s="54"/>
+      <c r="M16" s="45"/>
+      <c r="N16" s="46"/>
     </row>
     <row r="17" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="29"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="32"/>
-      <c r="M17" s="58"/>
-      <c r="N17" s="59"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="54"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="54"/>
+      <c r="J17" s="54"/>
+      <c r="K17" s="54"/>
+      <c r="L17" s="54"/>
+      <c r="M17" s="59"/>
+      <c r="N17" s="60"/>
     </row>
     <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="34"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="56"/>
-      <c r="N18" s="57"/>
+      <c r="A18" s="61"/>
+      <c r="B18" s="62"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="63"/>
+      <c r="E18" s="62"/>
+      <c r="F18" s="64"/>
+      <c r="G18" s="65"/>
+      <c r="H18" s="65"/>
+      <c r="I18" s="64"/>
+      <c r="J18" s="64"/>
+      <c r="K18" s="64"/>
+      <c r="L18" s="64"/>
+      <c r="M18" s="57"/>
+      <c r="N18" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="A5:M5"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="F6:M6"/>
-    <mergeCell ref="F7:M7"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="F8:M8"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="F9:M9"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="F10:M10"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="K18:L18"/>
     <mergeCell ref="M16:N16"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="D15:E15"/>
@@ -1877,18 +1890,23 @@
     <mergeCell ref="F16:H16"/>
     <mergeCell ref="I16:J16"/>
     <mergeCell ref="K16:L16"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="F9:M9"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="F10:M10"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="F6:M6"/>
+    <mergeCell ref="F7:M7"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="F8:M8"/>
+    <mergeCell ref="A7:E7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F7:M7" r:id="rId1" display="https://asi-storage07.blr.allegisindia.com/svn/EASi_App-POC/trunk/EasiCab/Documents/Planning"/>
@@ -1900,19 +1918,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" style="4" customWidth="1"/>
     <col min="2" max="2" width="36.42578125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="31" style="4" customWidth="1"/>
-    <col min="4" max="4" width="38.85546875" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="4"/>
+    <col min="3" max="3" width="39" style="4" customWidth="1"/>
+    <col min="4" max="4" width="46.5703125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="4"/>
+    <col min="6" max="6" width="21.140625" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2003,18 +2023,18 @@
         <v>15</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="1" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>28</v>
@@ -2032,7 +2052,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
         <v>30</v>
       </c>
@@ -2040,167 +2060,196 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C18" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="66">
+        <v>42606</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="7" t="s">
+    </row>
+    <row r="19" spans="1:6" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="67" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="67"/>
+      <c r="E20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="67"/>
+      <c r="E21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B24" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B25" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+    <row r="26" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="5"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="5"/>
-    </row>
-    <row r="27" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="B26" s="5"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="5"/>
+    </row>
+    <row r="29" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+    <row r="30" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+    <row r="31" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+    <row r="32" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
+    <row r="33" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>18</v>
+        <v>1</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="41" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>25</v>
+        <v>1</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="42" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
+    <row r="45" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>26</v>
+        <v>1</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2208,15 +2257,17 @@
   <hyperlinks>
     <hyperlink ref="B8" r:id="rId1"/>
     <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B23" r:id="rId3"/>
+    <hyperlink ref="B25" r:id="rId3"/>
     <hyperlink ref="B13" r:id="rId4"/>
-    <hyperlink ref="B29" r:id="rId5"/>
-    <hyperlink ref="B35" r:id="rId6"/>
-    <hyperlink ref="B41" r:id="rId7"/>
-    <hyperlink ref="B47" r:id="rId8"/>
+    <hyperlink ref="B31" r:id="rId5"/>
+    <hyperlink ref="B37" r:id="rId6"/>
+    <hyperlink ref="B43" r:id="rId7"/>
+    <hyperlink ref="B49" r:id="rId8"/>
     <hyperlink ref="D17" r:id="rId9"/>
+    <hyperlink ref="F19" r:id="rId10"/>
+    <hyperlink ref="F21" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>